<commit_message>
Update name of KhoaVNA in report 1. Update project management plan from 19/05/2014 to 26/05/2014. Update error messages definition.
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Client Error Messages" sheetId="1" r:id="rId1"/>
@@ -1900,6 +1900,1651 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="4" width="46.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B158" s="3"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B160" s="3"/>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B162" s="3"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B164" s="3"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B166" s="3"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B167" s="3"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B168" s="3"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B169" s="3"/>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B170" s="3"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B171" s="3"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B174" s="3"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B176" s="3"/>
+      <c r="C176" s="3"/>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B177" s="3"/>
+      <c r="C177" s="3"/>
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B178" s="3"/>
+      <c r="C178" s="3"/>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B196" s="3"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B199" s="3"/>
+      <c r="C199" s="3"/>
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B201" s="5"/>
+      <c r="C201" s="5"/>
+      <c r="D201" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D201"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,1651 +3569,6 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B75" s="3"/>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" s="3"/>
-      <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B91" s="3"/>
-      <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B92" s="3"/>
-      <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B93" s="3"/>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B109" s="3"/>
-      <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B110" s="3"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B111" s="3"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B112" s="3"/>
-      <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B135" s="3"/>
-      <c r="C135" s="3"/>
-      <c r="D135" s="3"/>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B136" s="3"/>
-      <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B137" s="3"/>
-      <c r="C137" s="3"/>
-      <c r="D137" s="3"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B138" s="3"/>
-      <c r="C138" s="3"/>
-      <c r="D138" s="3"/>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B139" s="3"/>
-      <c r="C139" s="3"/>
-      <c r="D139" s="3"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B140" s="3"/>
-      <c r="C140" s="3"/>
-      <c r="D140" s="3"/>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B141" s="3"/>
-      <c r="C141" s="3"/>
-      <c r="D141" s="3"/>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B142" s="3"/>
-      <c r="C142" s="3"/>
-      <c r="D142" s="3"/>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B143" s="3"/>
-      <c r="C143" s="3"/>
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
-      <c r="D145" s="3"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B146" s="3"/>
-      <c r="C146" s="3"/>
-      <c r="D146" s="3"/>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B147" s="3"/>
-      <c r="C147" s="3"/>
-      <c r="D147" s="3"/>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B148" s="3"/>
-      <c r="C148" s="3"/>
-      <c r="D148" s="3"/>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B149" s="3"/>
-      <c r="C149" s="3"/>
-      <c r="D149" s="3"/>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B150" s="3"/>
-      <c r="C150" s="3"/>
-      <c r="D150" s="3"/>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B151" s="3"/>
-      <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B152" s="3"/>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="3"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B177" s="3"/>
-      <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B178" s="3"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="B183" s="3"/>
-      <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B184" s="3"/>
-      <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B189" s="3"/>
-      <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B195" s="3"/>
-      <c r="C195" s="3"/>
-      <c r="D195" s="3"/>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B196" s="3"/>
-      <c r="C196" s="3"/>
-      <c r="D196" s="3"/>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B197" s="3"/>
-      <c r="C197" s="3"/>
-      <c r="D197" s="3"/>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B198" s="3"/>
-      <c r="C198" s="3"/>
-      <c r="D198" s="3"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B199" s="3"/>
-      <c r="C199" s="3"/>
-      <c r="D199" s="3"/>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B200" s="3"/>
-      <c r="C200" s="3"/>
-      <c r="D200" s="3"/>
-    </row>
-    <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B201" s="5"/>
-      <c r="C201" s="5"/>
-      <c r="D201" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D201"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="3" max="4" width="46.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Add Client Error Message CEM003
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="416">
   <si>
     <t>Error ID</t>
   </si>
@@ -1417,6 +1417,81 @@
         <scheme val="minor"/>
       </rPr>
       <t>{2}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the maximum length</t>
+    </r>
+  </si>
+  <si>
+    <t>Max length is not valid</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0} không thể vượt quá {1} ký tự.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">With
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the name of the element.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{1}</t>
     </r>
     <r>
       <rPr>
@@ -1951,13 +2026,19 @@
         <v>412</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">

</xml_diff>

<commit_message>
Modify error message and update Home Model
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -1512,51 +1512,6 @@
   </si>
   <si>
     <r>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> hợp lệ không vượt quá </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{1}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ký tự."</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">With
 </t>
     </r>
@@ -1607,31 +1562,6 @@
   </si>
   <si>
     <r>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> không hợp lệ"</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">With
 </t>
     </r>
@@ -1660,47 +1590,13 @@
     <t>Field's value's existed already.</t>
   </si>
   <si>
-    <r>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> này đã được sử dụng"</t>
-    </r>
-  </si>
-  <si>
     <t>Field's value is not existed.</t>
   </si>
   <si>
-    <t>"{0} của bạn không đúng"</t>
-  </si>
-  <si>
     <t>Re-type password is blank.</t>
   </si>
   <si>
-    <t>"Mật khẩu mới phải được nhập 2 lần để xác nhận mật khẩu".</t>
-  </si>
-  <si>
     <t>Two field's values are duplicated.</t>
-  </si>
-  <si>
-    <t>"{0} phải khác {1}"</t>
   </si>
   <si>
     <t>With
@@ -1711,9 +1607,6 @@
     <t>Two field's values are different.</t>
   </si>
   <si>
-    <t>"{0} không trùng khớp"</t>
-  </si>
-  <si>
     <t>With
 {0} is the name of the element.</t>
   </si>
@@ -1721,9 +1614,6 @@
     <t>Drop down list required field is blank</t>
   </si>
   <si>
-    <t>"Xin hãy chọn {0}"</t>
-  </si>
-  <si>
     <t>With
 {0} is the name of the required element.</t>
   </si>
@@ -1731,9 +1621,6 @@
     <t>Image filed's expression is invalid</t>
   </si>
   <si>
-    <t>"Tập tin hình ảnh không đúng định dạng"</t>
-  </si>
-  <si>
     <t>Create hospital user's account</t>
   </si>
   <si>
@@ -1768,58 +1655,557 @@
     <t>Update account information</t>
   </si>
   <si>
-    <t>"Mật khẩu thay đổi thành công"</t>
-  </si>
-  <si>
     <t>Update password successfully</t>
   </si>
   <si>
-    <t>"Không thể kích hoạt. Vui lòng thử lại sau"</t>
-  </si>
-  <si>
     <t>Cannot activate/deactivate account due to database connection</t>
   </si>
   <si>
     <t>Add new doctor</t>
   </si>
   <si>
-    <t>"Bác sĩ mới được tạo thành công"</t>
-  </si>
-  <si>
     <t>Insert doctor's information successfully.</t>
   </si>
   <si>
     <t>Update doctor's basic information</t>
   </si>
   <si>
-    <t>"Cập nhật thông tin thành công"</t>
-  </si>
-  <si>
     <t>Update doctor's basic information successfully.</t>
   </si>
   <si>
     <t>Update doctor's work schedule</t>
   </si>
   <si>
-    <t>"Cập nhật lịch làm việc thành công"</t>
-  </si>
-  <si>
     <t>Update doctor's work schedule successfully.</t>
   </si>
   <si>
     <t>Search not found</t>
   </si>
   <si>
-    <t>"Tìm không thấy"</t>
-  </si>
-  <si>
     <t>Confirm notification</t>
   </si>
   <si>
-    <t>"Tin nhắn xác nhận đã được gửi theo số điện thoại đăng kí. Vui lòng xác nhận cuộc hẹn qua tin nhắn"</t>
-  </si>
-  <si>
     <t>confirm message when user make an appointment.</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mật khẩu mới phải được nhập 2 lần để xác nhận mật khẩu.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hợp lệ không vượt quá {1} ký tự.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>không hợp lệ.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>phải khác</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{1}.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0} không trùng khớp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Xin hãy chọn {0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>này đã được sử dụng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>của bạn không đúng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cập nhật lịch làm việc thành công.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cập nhật thông tin thành công.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Không có kết quả phù hợp.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bác sĩ mới được tạo thành công.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Không thể kích hoạt. Vui lòng thử lại sau.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mật khẩu thay đổi thành công.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tin nhắn xác nhận đã được gửi theo số điện thoại đăng kí. Vui lòng xác nhận cuộc hẹn qua tin nhắn.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tập tin hình ảnh không đúng định dạng. (JPEG, JPG, PNG, BMP)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2046,7 +2432,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2081,7 +2467,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2292,9 +2678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2381,10 +2765,10 @@
         <v>417</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>418</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2392,13 +2776,13 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>420</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2406,13 +2790,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>424</v>
+        <v>452</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2420,13 +2804,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>426</v>
+        <v>453</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2434,10 +2818,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -2446,13 +2830,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>430</v>
+        <v>449</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2460,13 +2844,13 @@
         <v>15</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>433</v>
+        <v>450</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2474,24 +2858,24 @@
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>436</v>
+        <v>451</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>439</v>
+        <v>461</v>
       </c>
       <c r="D14" s="3"/>
     </row>
@@ -4001,9 +4385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4045,13 +4427,13 @@
         <v>205</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4059,13 +4441,13 @@
         <v>206</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>444</v>
+        <v>459</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4076,10 +4458,10 @@
         <v>404</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4087,13 +4469,13 @@
         <v>208</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4101,13 +4483,13 @@
         <v>209</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,13 +4497,13 @@
         <v>210</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>455</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>456</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4129,10 +4511,10 @@
         <v>211</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -4141,13 +4523,13 @@
         <v>212</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>460</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update report 3 and use case review
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client Error Messages" sheetId="1" r:id="rId1"/>
@@ -2580,7 +2580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4275,7 +4275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Update error message file
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="460">
   <si>
     <t>Error ID</t>
   </si>
@@ -2097,6 +2097,34 @@
         <scheme val="minor"/>
       </rPr>
       <t>không tồn tại.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Update hospital status failed</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đã có lỗi xảy ra trong quá trình thay đổi trạng thái của {0}.</t>
     </r>
     <r>
       <rPr>
@@ -4276,7 +4304,7 @@
   <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4424,12 +4452,16 @@
         <v>437</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>459</v>
+      </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update use case for final report
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Client Error Messages" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="508">
   <si>
     <t>Error ID</t>
   </si>
@@ -2759,6 +2759,12 @@
   <si>
     <t>With
 {0} is a specific number.</t>
+  </si>
+  <si>
+    <t>"Tài khoản hiện đang tạm khóa, xin vui lòng liên hệ ban quản trị để mở khóa tài khoản."</t>
+  </si>
+  <si>
+    <t>Account is deactive</t>
   </si>
 </sst>
 </file>
@@ -3245,8 +3251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5028,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5203,12 +5209,16 @@
         <v>462</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>506</v>
+      </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update final report user case
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Client Error Messages" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="511">
   <si>
     <t>Error ID</t>
   </si>
@@ -2761,10 +2761,41 @@
 {0} is a specific number.</t>
   </si>
   <si>
-    <t>"Tài khoản hiện đang tạm khóa, xin vui lòng liên hệ ban quản trị để mở khóa tài khoản."</t>
-  </si>
-  <si>
     <t>Account is deactive</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tài khoản hiện đang tạm khóa, xin vui lòng liên hệ ban quản trị để mở khóa tài khoản.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>"Xin hãy nhập tên bác sĩ hoặc chọn một chuyên khoa."</t>
+  </si>
+  <si>
+    <t>Doctor name or speciality drop down list is blank</t>
+  </si>
+  <si>
+    <t>Applied for tab Danh sách bác sỹ in page Hospital Detail</t>
   </si>
 </sst>
 </file>
@@ -2913,7 +2944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2943,6 +2974,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3251,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,13 +3730,19 @@
         <v>505</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>508</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
@@ -5034,8 +5074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5214,10 +5254,10 @@
         <v>214</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>506</v>
       </c>
       <c r="D13" s="3"/>
     </row>

</xml_diff>

<commit_message>
Update use case of final document
</commit_message>
<xml_diff>
--- a/Design/Error Message.xlsx
+++ b/Design/Error Message.xlsx
@@ -1952,51 +1952,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>{0}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>này đã được sử dụng.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"</t>
-    </r>
-  </si>
-  <si>
     <t>Field's value is already existed</t>
   </si>
   <si>
@@ -2796,6 +2751,51 @@
   </si>
   <si>
     <t>Applied for tab Danh sách bác sỹ in page Hospital Detail</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{0}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>đã được sử dụng.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3285,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3385,10 +3385,10 @@
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>448</v>
+        <v>510</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>417</v>
@@ -3399,10 +3399,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>417</v>
@@ -3413,7 +3413,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>437</v>
@@ -3425,7 +3425,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>439</v>
@@ -3439,10 +3439,10 @@
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>419</v>
@@ -3456,7 +3456,7 @@
         <v>420</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>421</v>
@@ -3479,10 +3479,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>419</v>
@@ -3493,10 +3493,10 @@
         <v>18</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>463</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>464</v>
       </c>
       <c r="D15" s="3"/>
     </row>
@@ -3505,10 +3505,10 @@
         <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>467</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>468</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -3517,10 +3517,10 @@
         <v>20</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>469</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>470</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -3529,10 +3529,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>471</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>472</v>
       </c>
       <c r="D18" s="3"/>
     </row>
@@ -3541,10 +3541,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>473</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>474</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -3553,10 +3553,10 @@
         <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>475</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>476</v>
       </c>
       <c r="D20" s="3"/>
     </row>
@@ -3565,10 +3565,10 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>477</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>478</v>
       </c>
       <c r="D21" s="3"/>
     </row>
@@ -3577,10 +3577,10 @@
         <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>480</v>
       </c>
       <c r="D22" s="3"/>
     </row>
@@ -3589,10 +3589,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>481</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>482</v>
       </c>
       <c r="D23" s="3"/>
     </row>
@@ -3601,10 +3601,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>484</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -3613,10 +3613,10 @@
         <v>28</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -3625,10 +3625,10 @@
         <v>29</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>487</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>488</v>
       </c>
       <c r="D26" s="3"/>
     </row>
@@ -3637,10 +3637,10 @@
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>490</v>
       </c>
       <c r="D27" s="3"/>
     </row>
@@ -3649,10 +3649,10 @@
         <v>31</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="D28" s="3"/>
     </row>
@@ -3661,10 +3661,10 @@
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>493</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>494</v>
       </c>
       <c r="D29" s="3"/>
     </row>
@@ -3673,10 +3673,10 @@
         <v>33</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>496</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -3685,10 +3685,10 @@
         <v>34</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>498</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -3697,10 +3697,10 @@
         <v>35</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D32" s="3"/>
     </row>
@@ -3709,10 +3709,10 @@
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D33" s="3"/>
     </row>
@@ -3721,13 +3721,13 @@
         <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3735,13 +3735,13 @@
         <v>38</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>507</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>509</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5220,7 +5220,7 @@
         <v>446</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5228,10 +5228,10 @@
         <v>212</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>455</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="D11" s="3"/>
     </row>
@@ -5240,13 +5240,13 @@
         <v>213</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>460</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5254,10 +5254,10 @@
         <v>214</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>506</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="D13" s="3"/>
     </row>

</xml_diff>